<commit_message>
Processing code as string (static dataset)
</commit_message>
<xml_diff>
--- a/src/data/data_processed/static_annual_data/air_pollution_reduction_systems_in_plants_by_voivodship.xlsx
+++ b/src/data/data_processed/static_annual_data/air_pollution_reduction_systems_in_plants_by_voivodship.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3229,8 +3229,10 @@
       <c r="A6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B6" t="n">
-        <v>200000</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0200000</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -3872,8 +3874,10 @@
       <c r="A7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B7" t="n">
-        <v>400000</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0400000</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -4515,8 +4519,10 @@
       <c r="A8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B8" t="n">
-        <v>600000</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0600000</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -5158,8 +5164,10 @@
       <c r="A9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B9" t="n">
-        <v>800000</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0800000</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -5801,8 +5809,10 @@
       <c r="A10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
-        <v>1000000</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1000000</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -6444,8 +6454,10 @@
       <c r="A11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B11" t="n">
-        <v>1200000</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1200000</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -7087,8 +7099,10 @@
       <c r="A12" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B12" t="n">
-        <v>1400000</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1400000</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -7730,8 +7744,10 @@
       <c r="A13" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B13" t="n">
-        <v>1600000</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1600000</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -8373,8 +8389,10 @@
       <c r="A14" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B14" t="n">
-        <v>1800000</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1800000</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -9016,8 +9034,10 @@
       <c r="A15" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B15" t="n">
-        <v>2000000</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2000000</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -9659,8 +9679,10 @@
       <c r="A16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B16" t="n">
-        <v>2200000</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2200000</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -10302,8 +10324,10 @@
       <c r="A17" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B17" t="n">
-        <v>2400000</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2400000</t>
+        </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -10945,8 +10969,10 @@
       <c r="A18" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B18" t="n">
-        <v>2600000</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2600000</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -11588,8 +11614,10 @@
       <c r="A19" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B19" t="n">
-        <v>2800000</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2800000</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -12231,8 +12259,10 @@
       <c r="A20" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B20" t="n">
-        <v>3000000</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>3000000</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -12874,8 +12904,10 @@
       <c r="A21" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B21" t="n">
-        <v>3200000</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>3200000</t>
+        </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>

</xml_diff>